<commit_message>
added webdriver listner and screehot
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/CRMNaveen.xlsx
+++ b/src/main/java/com/crm/qa/testdata/CRMNaveen.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DLL\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="6135"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>FirstName</t>
   </si>
@@ -38,9 +31,6 @@
     <t>Company</t>
   </si>
   <si>
-    <t>Mr.</t>
-  </si>
-  <si>
     <t>Ashutosh</t>
   </si>
   <si>
@@ -50,9 +40,6 @@
     <t>Genpact</t>
   </si>
   <si>
-    <t>Dr.</t>
-  </si>
-  <si>
     <t>Madhawan</t>
   </si>
   <si>
@@ -62,16 +49,10 @@
     <t>apollo</t>
   </si>
   <si>
-    <t>Er.</t>
-  </si>
-  <si>
     <t>Rahul</t>
   </si>
   <si>
     <t>Google</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Er. </t>
   </si>
   <si>
     <t>Reenika</t>
@@ -398,13 +379,13 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -417,64 +398,49 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>